<commit_message>
Started conversion to string process
</commit_message>
<xml_diff>
--- a/RoperALZDataMigration/RoperSpreadSheet.xlsx
+++ b/RoperALZDataMigration/RoperSpreadSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trident\work\XferSpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\git\roper-alz-data-migration1\RoperALZDataMigration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9B72C3A2-A451-4480-9A46-1A374224F0AB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
+  <xr:revisionPtr documentId="13_ncr:1_{155FB899-7E79-4693-89B6-0B6AE0B99DB6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
     <workbookView windowHeight="12300" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
@@ -18,8 +18,8 @@
     <sheet name="OptInEamils" r:id="rId3" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable11">Table1[]</definedName>
-    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable21">Table2</definedName>
+    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable1">Table1[]</definedName>
+    <definedName hidden="1" name="_xlcn.WorksheetConnection_newdatabase.xlsxTable2">Table2</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -56,7 +56,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable11"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable21"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_newdatabase.xlsxTable2"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="148">
   <si>
     <t>Last Name</t>
   </si>
@@ -202,12 +202,18 @@
     <t>Column1</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>WELLS</t>
   </si>
   <si>
     <t>PATRICK</t>
   </si>
   <si>
+    <t>11/14/1938</t>
+  </si>
+  <si>
     <t>W</t>
   </si>
   <si>
@@ -226,7 +232,7 @@
     <t>9/10/14 - 29/25</t>
   </si>
   <si>
-    <t/>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Advantage Memory Screen Day</t>
@@ -238,6 +244,9 @@
     <t>DARREN</t>
   </si>
   <si>
+    <t>09/13/1943</t>
+  </si>
+  <si>
     <t>926 ABBEY ST Charleston, SC 29401</t>
   </si>
   <si>
@@ -262,6 +271,9 @@
     <t>JENNIE</t>
   </si>
   <si>
+    <t>11/12/1936</t>
+  </si>
+  <si>
     <t>101 ACACIA AVE Charleston, SC 29401</t>
   </si>
   <si>
@@ -286,6 +298,9 @@
     <t>AMY</t>
   </si>
   <si>
+    <t>03/27/1964</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -310,6 +325,9 @@
     <t>JANICE</t>
   </si>
   <si>
+    <t>05/07/1930</t>
+  </si>
+  <si>
     <t>149 ACACIA ST Charleston, SC 29401</t>
   </si>
   <si>
@@ -334,6 +352,9 @@
     <t>FELICIA</t>
   </si>
   <si>
+    <t>07/07/1959</t>
+  </si>
+  <si>
     <t>16 ACACIA ST Charleston, SC 29401</t>
   </si>
   <si>
@@ -358,6 +379,9 @@
     <t>JAY</t>
   </si>
   <si>
+    <t>07/06/1925</t>
+  </si>
+  <si>
     <t>515 ACADIA ST Charleston, SC 29401</t>
   </si>
   <si>
@@ -379,6 +403,9 @@
     <t>BETTY</t>
   </si>
   <si>
+    <t>07/19/1958</t>
+  </si>
+  <si>
     <t>465 ACADIA ST Charleston, SC 29401</t>
   </si>
   <si>
@@ -403,6 +430,9 @@
     <t>STACEY</t>
   </si>
   <si>
+    <t>04/07/1929</t>
+  </si>
+  <si>
     <t>972 ACEVEDO AVE Charleston, SC 29401</t>
   </si>
   <si>
@@ -421,6 +451,9 @@
     <t>PRISCILLA</t>
   </si>
   <si>
+    <t>09/13/1931</t>
+  </si>
+  <si>
     <t>777 ACEVEDO AVE Charleston, SC 29401</t>
   </si>
   <si>
@@ -445,6 +478,9 @@
     <t>VINCENT</t>
   </si>
   <si>
+    <t>11/03/1928</t>
+  </si>
+  <si>
     <t>974 ACME ALY Charleston, SC 29401</t>
   </si>
   <si>
@@ -464,6 +500,9 @@
   </si>
   <si>
     <t>MABEL</t>
+  </si>
+  <si>
+    <t>11/22/1942</t>
   </si>
   <si>
     <t>454 ACME ALY Charleston, SC 29401</t>
@@ -485,8 +524,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="165" formatCode="MM/dd/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -517,24 +557,50 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt formatCode="m/d/yyyy" numFmtId="19"/>
-    </dxf>
-    <dxf>
       <numFmt formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####" numFmtId="164"/>
     </dxf>
     <dxf>
       <numFmt formatCode="0.00" numFmtId="2"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="m/d/yyyy" numFmtId="19"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
@@ -555,13 +621,13 @@
   <tableColumns count="13">
     <tableColumn id="1" name="Last Name" xr3:uid="{00000000-0010-0000-0000-000001000000}"/>
     <tableColumn id="2" name="First Name" xr3:uid="{00000000-0010-0000-0000-000002000000}"/>
-    <tableColumn dataDxfId="0" id="3" name="DOB" xr3:uid="{00000000-0010-0000-0000-000003000000}"/>
-    <tableColumn dataDxfId="2" id="4" name="age" xr3:uid="{00000000-0010-0000-0000-000004000000}"/>
+    <tableColumn dataDxfId="2" id="3" name="DOB" xr3:uid="{00000000-0010-0000-0000-000003000000}"/>
+    <tableColumn dataDxfId="1" id="4" name="age" xr3:uid="{00000000-0010-0000-0000-000004000000}"/>
     <tableColumn id="5" name="Race" xr3:uid="{00000000-0010-0000-0000-000005000000}"/>
     <tableColumn id="6" name="Gender" xr3:uid="{00000000-0010-0000-0000-000006000000}"/>
     <tableColumn id="7" name="Address" xr3:uid="{00000000-0010-0000-0000-000007000000}"/>
     <tableColumn id="8" name="Email Address" xr3:uid="{00000000-0010-0000-0000-000008000000}"/>
-    <tableColumn dataDxfId="1" id="9" name="Phone Number" xr3:uid="{00000000-0010-0000-0000-000009000000}"/>
+    <tableColumn dataDxfId="0" id="9" name="Phone Number" xr3:uid="{00000000-0010-0000-0000-000009000000}"/>
     <tableColumn id="10" name="PCP" xr3:uid="{00000000-0010-0000-0000-00000A000000}"/>
     <tableColumn id="11" name="Specialist" xr3:uid="{00000000-0010-0000-0000-00000B000000}"/>
     <tableColumn id="12" name="Referral" xr3:uid="{00000000-0010-0000-0000-00000C000000}"/>
@@ -844,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R28"/>
+  <dimension ref="B1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +932,7 @@
     <col min="14" max="14" customWidth="true" width="20.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -907,312 +973,310 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="J2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="n">
-        <v>14198.0</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D3"/>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="n">
-        <v>15962.0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" t="s">
+      <c r="Q5" t="s">
         <v>61</v>
-      </c>
-      <c r="D5" t="n">
-        <v>13466.0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" t="n">
-        <v>23463.0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="Q6" t="s">
         <v>70</v>
-      </c>
-      <c r="H6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" t="n">
-        <v>11085.0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>78</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" t="s">
         <v>79</v>
-      </c>
-      <c r="J7" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" t="s">
+      <c r="I8" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="n">
-        <v>21738.0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>86</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" t="s">
         <v>87</v>
       </c>
-      <c r="J8" t="s">
+      <c r="Q8" t="s">
         <v>88</v>
-      </c>
-      <c r="K8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P8" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
         <v>92</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
         <v>93</v>
       </c>
-      <c r="D9" t="n">
-        <v>9319.0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>94</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>95</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
         <v>96</v>
-      </c>
-      <c r="K9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" t="s">
-        <v>98</v>
-      </c>
-      <c r="N9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P9" t="s">
-        <v>50</v>
       </c>
       <c r="Q9" t="s">
         <v>97</v>
@@ -1225,38 +1289,38 @@
       <c r="C10" t="s">
         <v>100</v>
       </c>
-      <c r="D10" t="n">
-        <v>21385.0</v>
+      <c r="D10" t="s">
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" t="s">
         <v>106</v>
       </c>
-      <c r="L10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10" t="s">
-        <v>26</v>
-      </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P10" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="Q10" t="s">
         <v>105</v>
@@ -1269,520 +1333,522 @@
       <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="D11" t="n">
-        <v>10690.0</v>
+      <c r="D11" t="s">
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="L11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="P11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q11" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" t="n">
-        <v>11579.0</v>
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I12" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J12" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P12" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Q12" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" t="n">
-        <v>10535.0</v>
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I13" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="N13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="Q13" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" t="n">
-        <v>15667.0</v>
+        <v>133</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="I14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" t="s">
+        <v>137</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" t="s">
         <v>131</v>
       </c>
-      <c r="J14" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" t="s">
-        <v>50</v>
-      </c>
-      <c r="L14" t="s">
-        <v>50</v>
-      </c>
-      <c r="M14" t="s">
-        <v>26</v>
-      </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P14" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="Q14" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15"/>
+        <v>141</v>
+      </c>
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="K15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M15" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="N15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="P15" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="Q15" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="n">
-        <v>14198.0</v>
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="Q16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="n">
-        <v>15962.0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" t="s">
-        <v>32</v>
-      </c>
       <c r="N17" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="Q17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>62</v>
+      </c>
+      <c r="P18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
+      <c r="Q18" t="s">
         <v>61</v>
-      </c>
-      <c r="D18" t="n">
-        <v>13466.0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18" t="s">
-        <v>50</v>
-      </c>
-      <c r="N18" t="s">
-        <v>50</v>
-      </c>
-      <c r="P18" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="n">
-        <v>23463.0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="Q19" t="s">
         <v>70</v>
-      </c>
-      <c r="H19" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L19" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" t="s">
-        <v>59</v>
-      </c>
-      <c r="P19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="I20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" t="n">
-        <v>11085.0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>78</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>62</v>
+      </c>
+      <c r="P20" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q20" t="s">
         <v>79</v>
-      </c>
-      <c r="J20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K20" t="s">
-        <v>83</v>
-      </c>
-      <c r="L20" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N20" t="s">
-        <v>50</v>
-      </c>
-      <c r="P20" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
+      <c r="I21" t="s">
         <v>85</v>
       </c>
-      <c r="D21" t="n">
-        <v>21738.0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>86</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
+        <v>89</v>
+      </c>
+      <c r="L21" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" t="s">
+        <v>52</v>
+      </c>
+      <c r="P21" t="s">
         <v>87</v>
       </c>
-      <c r="J21" t="s">
+      <c r="Q21" t="s">
         <v>88</v>
-      </c>
-      <c r="K21" t="s">
-        <v>91</v>
-      </c>
-      <c r="L21" t="s">
-        <v>50</v>
-      </c>
-      <c r="M21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21" t="s">
-        <v>59</v>
-      </c>
-      <c r="P21" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
         <v>92</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
         <v>93</v>
       </c>
-      <c r="D22" t="n">
-        <v>9319.0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>94</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" t="s">
         <v>96</v>
-      </c>
-      <c r="K22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" t="s">
-        <v>50</v>
-      </c>
-      <c r="M22" t="s">
-        <v>98</v>
-      </c>
-      <c r="N22" t="s">
-        <v>50</v>
-      </c>
-      <c r="P22" t="s">
-        <v>50</v>
       </c>
       <c r="Q22" t="s">
         <v>97</v>
@@ -1795,38 +1861,38 @@
       <c r="C23" t="s">
         <v>100</v>
       </c>
-      <c r="D23" t="n">
-        <v>21385.0</v>
+      <c r="D23" t="s">
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" t="s">
         <v>106</v>
       </c>
-      <c r="L23" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" t="s">
-        <v>26</v>
-      </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P23" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="Q23" t="s">
         <v>105</v>
@@ -1839,215 +1905,261 @@
       <c r="C24" t="s">
         <v>108</v>
       </c>
-      <c r="D24" t="n">
-        <v>10690.0</v>
+      <c r="D24" t="s">
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K24" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="L24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M24" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="P24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q24" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" t="n">
-        <v>11579.0</v>
+        <v>117</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J25" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="K25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M25" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="N25" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P25" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Q25" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" t="n">
-        <v>10535.0</v>
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
+        <v>125</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="H26" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J26" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M26" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="N26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P26" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="Q26" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" t="n">
-        <v>15667.0</v>
+        <v>133</v>
+      </c>
+      <c r="D27" t="s">
+        <v>134</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H27" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="I27" t="s">
+        <v>136</v>
+      </c>
+      <c r="J27" t="s">
+        <v>137</v>
+      </c>
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" t="s">
+        <v>52</v>
+      </c>
+      <c r="M27" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
-        <v>132</v>
-      </c>
-      <c r="K27" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" t="s">
-        <v>50</v>
-      </c>
-      <c r="M27" t="s">
-        <v>26</v>
-      </c>
       <c r="N27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P27" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="Q27" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28"/>
+        <v>141</v>
+      </c>
+      <c r="D28" t="s">
+        <v>142</v>
+      </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="I28" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="J28" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="K28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M28" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="P28" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="Q28" t="s">
-        <v>50</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" t="s">
+        <v>52</v>
+      </c>
+      <c r="K29" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" t="s">
+        <v>52</v>
+      </c>
+      <c r="P29" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the reader added creatWorkbook method and getNextRecord method
</commit_message>
<xml_diff>
--- a/RoperALZDataMigration/RoperSpreadSheet.xlsx
+++ b/RoperALZDataMigration/RoperSpreadSheet.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="148">
   <si>
     <t>Last Name</t>
   </si>
@@ -557,11 +557,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
@@ -923,7 +936,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R42"/>
+  <dimension ref="B1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -2744,6 +2757,578 @@
         <v>52</v>
       </c>
       <c r="Q42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" t="s">
+        <v>49</v>
+      </c>
+      <c r="J43" t="s">
+        <v>50</v>
+      </c>
+      <c r="K43" t="s">
+        <v>52</v>
+      </c>
+      <c r="L43" t="s">
+        <v>52</v>
+      </c>
+      <c r="M43" t="s">
+        <v>53</v>
+      </c>
+      <c r="N43" t="s">
+        <v>52</v>
+      </c>
+      <c r="P43" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I44" t="s">
+        <v>58</v>
+      </c>
+      <c r="J44" t="s">
+        <v>59</v>
+      </c>
+      <c r="K44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L44" t="s">
+        <v>52</v>
+      </c>
+      <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>62</v>
+      </c>
+      <c r="P44" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I45" t="s">
+        <v>67</v>
+      </c>
+      <c r="J45" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" t="s">
+        <v>71</v>
+      </c>
+      <c r="L45" t="s">
+        <v>52</v>
+      </c>
+      <c r="M45" t="s">
+        <v>52</v>
+      </c>
+      <c r="N45" t="s">
+        <v>52</v>
+      </c>
+      <c r="P45" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>77</v>
+      </c>
+      <c r="J46" t="s">
+        <v>78</v>
+      </c>
+      <c r="K46" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46" t="s">
+        <v>52</v>
+      </c>
+      <c r="M46" t="s">
+        <v>28</v>
+      </c>
+      <c r="N46" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47" t="s">
+        <v>84</v>
+      </c>
+      <c r="I47" t="s">
+        <v>85</v>
+      </c>
+      <c r="J47" t="s">
+        <v>86</v>
+      </c>
+      <c r="K47" t="s">
+        <v>89</v>
+      </c>
+      <c r="L47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M47" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" t="s">
+        <v>52</v>
+      </c>
+      <c r="P47" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
+      <c r="I48" t="s">
+        <v>94</v>
+      </c>
+      <c r="J48" t="s">
+        <v>95</v>
+      </c>
+      <c r="K48" t="s">
+        <v>98</v>
+      </c>
+      <c r="L48" t="s">
+        <v>52</v>
+      </c>
+      <c r="M48" t="s">
+        <v>24</v>
+      </c>
+      <c r="N48" t="s">
+        <v>62</v>
+      </c>
+      <c r="P48" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" t="s">
+        <v>102</v>
+      </c>
+      <c r="I49" t="s">
+        <v>103</v>
+      </c>
+      <c r="J49" t="s">
+        <v>104</v>
+      </c>
+      <c r="K49" t="s">
+        <v>52</v>
+      </c>
+      <c r="L49" t="s">
+        <v>52</v>
+      </c>
+      <c r="M49" t="s">
+        <v>106</v>
+      </c>
+      <c r="N49" t="s">
+        <v>52</v>
+      </c>
+      <c r="P49" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50" t="s">
+        <v>47</v>
+      </c>
+      <c r="H50" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" t="s">
+        <v>111</v>
+      </c>
+      <c r="J50" t="s">
+        <v>112</v>
+      </c>
+      <c r="K50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L50" t="s">
+        <v>52</v>
+      </c>
+      <c r="M50" t="s">
+        <v>26</v>
+      </c>
+      <c r="N50" t="s">
+        <v>62</v>
+      </c>
+      <c r="P50" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" t="s">
+        <v>119</v>
+      </c>
+      <c r="I51" t="s">
+        <v>120</v>
+      </c>
+      <c r="J51" t="s">
+        <v>121</v>
+      </c>
+      <c r="K51" t="s">
+        <v>52</v>
+      </c>
+      <c r="L51" t="s">
+        <v>52</v>
+      </c>
+      <c r="M51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N51" t="s">
+        <v>52</v>
+      </c>
+      <c r="P51" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" t="s">
+        <v>75</v>
+      </c>
+      <c r="H52" t="s">
+        <v>126</v>
+      </c>
+      <c r="I52" t="s">
+        <v>127</v>
+      </c>
+      <c r="J52" t="s">
+        <v>128</v>
+      </c>
+      <c r="K52" t="s">
+        <v>52</v>
+      </c>
+      <c r="L52" t="s">
+        <v>52</v>
+      </c>
+      <c r="M52" t="s">
+        <v>131</v>
+      </c>
+      <c r="N52" t="s">
+        <v>62</v>
+      </c>
+      <c r="P52" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53" t="s">
+        <v>47</v>
+      </c>
+      <c r="H53" t="s">
+        <v>135</v>
+      </c>
+      <c r="I53" t="s">
+        <v>136</v>
+      </c>
+      <c r="J53" t="s">
+        <v>137</v>
+      </c>
+      <c r="K53" t="s">
+        <v>52</v>
+      </c>
+      <c r="L53" t="s">
+        <v>52</v>
+      </c>
+      <c r="M53" t="s">
+        <v>131</v>
+      </c>
+      <c r="N53" t="s">
+        <v>62</v>
+      </c>
+      <c r="P53" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" t="s">
+        <v>143</v>
+      </c>
+      <c r="I54" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54" t="s">
+        <v>145</v>
+      </c>
+      <c r="K54" t="s">
+        <v>52</v>
+      </c>
+      <c r="L54" t="s">
+        <v>52</v>
+      </c>
+      <c r="M54" t="s">
+        <v>26</v>
+      </c>
+      <c r="N54" t="s">
+        <v>62</v>
+      </c>
+      <c r="P54" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I55" t="s">
+        <v>52</v>
+      </c>
+      <c r="J55" t="s">
+        <v>52</v>
+      </c>
+      <c r="K55" t="s">
+        <v>52</v>
+      </c>
+      <c r="L55" t="s">
+        <v>52</v>
+      </c>
+      <c r="M55" t="s">
+        <v>52</v>
+      </c>
+      <c r="N55" t="s">
+        <v>52</v>
+      </c>
+      <c r="P55" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q55" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>